<commit_message>
Add to reading notes
</commit_message>
<xml_diff>
--- a/inst/ms/reading.xlsx
+++ b/inst/ms/reading.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23416"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14840" tabRatio="500"/>
+    <workbookView xWindow="-25980" yWindow="15640" windowWidth="25600" windowHeight="14840" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="113">
   <si>
     <t>Author</t>
   </si>
@@ -72,9 +72,6 @@
     <t>biocomplexity</t>
   </si>
   <si>
-    <t>Maintainance of biocomplexity (a diversity of life-history strategies) an important component of long-term sustainability; specifically, they show that not all sockeye in Bristol Bay respond similarly to the environment</t>
-  </si>
-  <si>
     <t>We believe that long-term sustainability is derived in large part from com- plementary patterns of productivity in different stock components; It would seem prudent to try to prevent loss of such stock components, including those that appear, at present, to be unproductive.</t>
   </si>
   <si>
@@ -144,12 +141,6 @@
     <t>Defines response diversity; states that it's important to resilience; provides "adaptive capacity"</t>
   </si>
   <si>
-    <t>Liebhold</t>
-  </si>
-  <si>
-    <t>Spatial synchrony can occur because of: (1) dispersal between populations (2) Moran effect, (3) trophic interactions with other pops that are synchronous</t>
-  </si>
-  <si>
     <t>Moore</t>
   </si>
   <si>
@@ -190,6 +181,183 @@
   </si>
   <si>
     <t>Hodgson</t>
+  </si>
+  <si>
+    <t>"only 0.25% of the papers on conservation and/or management of salmonids list the keyword "metapopulation""</t>
+  </si>
+  <si>
+    <t>Levins</t>
+  </si>
+  <si>
+    <t>First paper to coin term metapopulation</t>
+  </si>
+  <si>
+    <t>Second paper to coin term metapopulation</t>
+  </si>
+  <si>
+    <t>Gilpin and Hanski</t>
+  </si>
+  <si>
+    <t>The book that set off metapopulation biology</t>
+  </si>
+  <si>
+    <t>Maintainance of biocomplexity (a diversity of life-history strategies) an important component of long-term sustainability; specifically, they show that not all sockeye in Bristol Bay respond similarly to the environment. And, fishing causes less variability than natural processes.</t>
+  </si>
+  <si>
+    <t>metapopulations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Peterman et al. </t>
+  </si>
+  <si>
+    <t>Stewart et al.</t>
+  </si>
+  <si>
+    <t>2003a</t>
+  </si>
+  <si>
+    <t>from Schtickzelle: correlations between pops up to 175km apartnegative -.55 to 1.00 in survival</t>
+  </si>
+  <si>
+    <t>Isaak et al</t>
+  </si>
+  <si>
+    <t>Kindvall</t>
+  </si>
+  <si>
+    <t>(1) habitat heterogeneity can create different responses to the same conditions (for bush cricket metapopulations) and (2) extinction risk higher in homogenous habitats</t>
+  </si>
+  <si>
+    <t>environmental filter</t>
+  </si>
+  <si>
+    <t>(1) salmon metapops become more synchronized at low abundance and (2) dispersal unlikely to affect population dynamics unless abundance really low where it can synchronize</t>
+  </si>
+  <si>
+    <t>Liebhold et al.</t>
+  </si>
+  <si>
+    <t>Spatial synchrony can occur because of: (1) dispersal between populations (2) Moran effect, (3) trophic interactions with other pops that are synchronous; shared environment and dispersal more likely for closer pops</t>
+  </si>
+  <si>
+    <t>Quinn (book)</t>
+  </si>
+  <si>
+    <t>Main pacific salmon reference. One point: Because anadromous salmon pops spend time together in ocean, even if far apart in freshwater experience same environment in ocean, and so correlation may decay less than you'd think with distance</t>
+  </si>
+  <si>
+    <t>Hindar et al.</t>
+  </si>
+  <si>
+    <t>genetic variation</t>
+  </si>
+  <si>
+    <t>The genetic consequences of harvesting need to be assessed both at the levels of local populations and the metapopulation.</t>
+  </si>
+  <si>
+    <t>Waples</t>
+  </si>
+  <si>
+    <t>TO GET: effective size of fluctuating…</t>
+  </si>
+  <si>
+    <t>Cooper and Mangel</t>
+  </si>
+  <si>
+    <t>Dangerous to ignore metapopulation structure of salmon</t>
+  </si>
+  <si>
+    <t>Frankham</t>
+  </si>
+  <si>
+    <t>TO GET: inbreeding and extinction a threshold effect</t>
+  </si>
+  <si>
+    <t>Lande and Shannon</t>
+  </si>
+  <si>
+    <t>TO GET: the role of genetic variation in adaptation…</t>
+  </si>
+  <si>
+    <t>Moritz</t>
+  </si>
+  <si>
+    <t>ESU</t>
+  </si>
+  <si>
+    <t>TO GET: defining 'evolutionarily significant units' for conservation TREE</t>
+  </si>
+  <si>
+    <t>Pulliam</t>
+  </si>
+  <si>
+    <t>sources and sinks</t>
+  </si>
+  <si>
+    <t>TO GET: sources, sinks, and population regulation</t>
+  </si>
+  <si>
+    <t>Ryman et al.</t>
+  </si>
+  <si>
+    <t>TO GET: protection of intraspecific biodiversity…</t>
+  </si>
+  <si>
+    <t>Taylor</t>
+  </si>
+  <si>
+    <t>local adaptation</t>
+  </si>
+  <si>
+    <t>TO GET: a review of local adaptation in salmonidae</t>
+  </si>
+  <si>
+    <t>Defines ESUs</t>
+  </si>
+  <si>
+    <t>TO GET</t>
+  </si>
+  <si>
+    <t>Mace and Lande</t>
+  </si>
+  <si>
+    <t>TO GET: assessing extinction threats: towards a genetically secure population</t>
+  </si>
+  <si>
+    <t>Wang et al.</t>
+  </si>
+  <si>
+    <t>inbreeding</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TO GET: salmonid inbreeding: a review </t>
+  </si>
+  <si>
+    <t>need to consider genetic effects of harvesting both at local and metapopulation level</t>
+  </si>
+  <si>
+    <t>Fahrig</t>
+  </si>
+  <si>
+    <t>habitat fragmentation</t>
+  </si>
+  <si>
+    <t>TO GET: effects of habitat fragementation on biodiversity</t>
+  </si>
+  <si>
+    <t>Hanski</t>
+  </si>
+  <si>
+    <t>TO GET: metapopulation dynamics: does it help to have more….</t>
+  </si>
+  <si>
+    <t>Baguette</t>
+  </si>
+  <si>
+    <t>Anadromous salmon likely fulfill the 3 requirements to be defined as a metapopulation: discrete populations, some asynchrony; some dispersal. Useful concept, but, the concept is rarely used or tested. Main implications: (1) metapop dynamics can influence persistence or collapse (ecological time scale) and (2) evolution and adaptation (evolutionary time scale); dispersal likely just enough to "ensure recolonization of suitable habitat"; salmon tend to stray near their natal stream, although not necessarily those closest</t>
+  </si>
+  <si>
+    <t>Basically, we need to loosen up on "classical metapopulation theory" for it to be useful. Classical definition is rare and maybe not always applicable to conservation or empirical work</t>
   </si>
 </sst>
 </file>
@@ -564,18 +732,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F27"/>
+  <dimension ref="A1:F49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="13.1640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="6.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="59.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="54.33203125" style="1" customWidth="1"/>
     <col min="5" max="5" width="64.1640625" style="1" customWidth="1"/>
     <col min="6" max="6" width="31.1640625" style="1" customWidth="1"/>
   </cols>
@@ -645,7 +813,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="60">
+    <row r="5" spans="1:5" ht="75">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -656,15 +824,15 @@
         <v>16</v>
       </c>
       <c r="D5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="30">
       <c r="A6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B6" s="2">
         <v>2008</v>
@@ -673,12 +841,12 @@
         <v>6</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="30">
       <c r="A7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B7" s="2">
         <v>1997</v>
@@ -687,92 +855,101 @@
         <v>6</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="60">
       <c r="A8" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="2">
         <v>1997</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="75">
       <c r="A9" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2">
         <v>2007</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D9" s="1" t="s">
+    </row>
+    <row r="10" spans="1:5" ht="75">
+      <c r="A10" s="1" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="60">
-      <c r="A10" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="B10" s="2">
         <v>1993</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="45">
       <c r="A11" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B11" s="2">
         <v>2011</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="E11" s="1" t="s">
+    </row>
+    <row r="12" spans="1:5" ht="135">
+      <c r="A12" s="1" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5">
-      <c r="A12" s="1" t="s">
-        <v>34</v>
       </c>
       <c r="B12" s="2">
         <v>2007</v>
       </c>
+      <c r="C12" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13" s="2">
         <v>2011</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="30">
+    <row r="14" spans="1:5">
       <c r="A14" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B14" s="2">
         <v>2000</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B15" s="2">
         <v>2003</v>
@@ -780,29 +957,29 @@
     </row>
     <row r="16" spans="1:5" ht="30">
       <c r="A16" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B16" s="2">
         <v>2003</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="45">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="60">
       <c r="A17" s="1" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="B17" s="2">
         <v>2004</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>42</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:6">
       <c r="A18" s="1" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B18" s="2">
         <v>2010</v>
@@ -810,69 +987,358 @@
     </row>
     <row r="19" spans="1:6" ht="75">
       <c r="A19" s="1" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B19" s="2">
         <v>1972</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="90">
       <c r="A20" s="1" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B20" s="2">
         <v>1991</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="30">
       <c r="A21" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B21" s="2">
         <v>1968</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="60">
+      <c r="A22" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B22" s="2">
+        <v>2005</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="26" spans="1:6">
       <c r="A26" s="1" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B26" s="2">
         <v>2008</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:6">
       <c r="A27" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="B27" s="2">
         <v>2002</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="1" t="s">
         <v>55</v>
+      </c>
+      <c r="B28" s="2">
+        <v>1969</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="2">
+        <v>1970</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30">
+      <c r="A30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B30" s="2">
+        <v>1991</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="30">
+      <c r="A31" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B31" s="2">
+        <v>1998</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="30">
+      <c r="A32" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" ht="45">
+      <c r="A33" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B33" s="2">
+        <v>2003</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" ht="45">
+      <c r="A34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="2">
+        <v>1996</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" ht="30">
+      <c r="A35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="2">
+        <v>2004</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" ht="45">
+      <c r="A36" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B36" s="2">
+        <v>2002</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" ht="30">
+      <c r="A37" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="2">
+        <v>1999</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" ht="60">
+      <c r="A38" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="B38" s="2">
+        <v>1995</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="30">
+      <c r="A39" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B39" s="2">
+        <v>1996</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" ht="30">
+      <c r="A40" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B40" s="2">
+        <v>1994</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" ht="30">
+      <c r="A41" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B41" s="2">
+        <v>1988</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5">
+      <c r="A42" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B42" s="2">
+        <v>1995</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5">
+      <c r="A43" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B43" s="2">
+        <v>1991</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5">
+      <c r="A44" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="B44" s="2">
+        <v>1991</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="105">
+      <c r="A45" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B45" s="2">
+        <v>1991</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5">
+      <c r="A46" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B46" s="2">
+        <v>2002</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="30">
+      <c r="A47" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B47" s="2">
+        <v>2003</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5">
+      <c r="A48" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B48" s="2">
+        <v>1998</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="45">
+      <c r="A49" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="B49" s="2">
+        <v>2004</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>